<commit_message>
updates to pintle design documentation
</commit_message>
<xml_diff>
--- a/V_Series/Pintle_V3_Testing raw data/Data Analysis Summary.xlsx
+++ b/V_Series/Pintle_V3_Testing raw data/Data Analysis Summary.xlsx
@@ -5,33 +5,34 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jntil\Documents\Git_Repos\pintle-injector\Pintle_V3_Testing raw data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jntil\Documents\Git_Repos\pintle-injector\V_Series\Pintle_V3_Testing raw data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04205747-A647-4D63-85EF-EAEB94ED6BAA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7F2BD1-CB37-4A8C-A475-40D7379F3D84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="960" windowWidth="12240" windowHeight="9720" xr2:uid="{1C337766-0B60-4982-99F7-C0C8567B4E66}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{1C337766-0B60-4982-99F7-C0C8567B4E66}"/>
   </bookViews>
   <sheets>
     <sheet name="FlowRate" sheetId="2" r:id="rId1"/>
     <sheet name="Fow Rates Raw" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Annulus_area">FlowRate!$Z$5</definedName>
+    <definedName name="Annulus_area">FlowRate!$Z$6</definedName>
     <definedName name="annulus_area2">FlowRate!$AE$6</definedName>
     <definedName name="blockage_factor">FlowRate!$AF$3</definedName>
-    <definedName name="Density_h20">FlowRate!$B$4</definedName>
-    <definedName name="density_IPA">FlowRate!$AI$32</definedName>
-    <definedName name="density_LOX">FlowRate!$AI$31</definedName>
-    <definedName name="gal_to_meter">FlowRate!$C$7</definedName>
+    <definedName name="Density_h20">FlowRate!$X$5</definedName>
+    <definedName name="density_IPA">FlowRate!$X$7</definedName>
+    <definedName name="density_LOX">FlowRate!$X$6</definedName>
+    <definedName name="gal_to_meter">FlowRate!$Y$3</definedName>
+    <definedName name="gap">FlowRate!$AC$6</definedName>
     <definedName name="kl_annulus">FlowRate!$Z$15</definedName>
     <definedName name="kl_pintle">FlowRate!$Z$23</definedName>
-    <definedName name="Liter_to_meter">FlowRate!$C$4</definedName>
-    <definedName name="Pintle_Area">FlowRate!$Z$4</definedName>
+    <definedName name="Liter_to_meter">FlowRate!$X$3</definedName>
+    <definedName name="orifice">FlowRate!$AD$6</definedName>
+    <definedName name="Pintle_Area">FlowRate!$Z$5</definedName>
     <definedName name="pintle_area2">FlowRate!$AC$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="73">
   <si>
     <t>Annulus</t>
   </si>
@@ -260,17 +261,25 @@
   </si>
   <si>
     <t>With current geometry, experimental KL value, these 'should' be the target pressures for using LOX and IPA to get the mass flow rates, and momentum ratio of 1</t>
+  </si>
+  <si>
+    <t>Values used for other equations in spreadsheet</t>
+  </si>
+  <si>
+    <t>density h20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="0.000000"/>
+    <numFmt numFmtId="172" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,8 +294,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,8 +346,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -338,12 +367,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -391,7 +500,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -409,6 +517,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -416,6 +527,83 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -733,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBDD6AF2-C968-43EC-BB41-EAA96344CA84}">
-  <dimension ref="A2:AM67"/>
+  <dimension ref="A1:AM67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="R22" workbookViewId="0">
+      <selection activeCell="AE25" sqref="AE25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,27 +932,52 @@
     <col min="5" max="5" width="9.140625" style="1"/>
     <col min="6" max="18" width="6.85546875" style="1" customWidth="1"/>
     <col min="19" max="19" width="5.140625" customWidth="1"/>
-    <col min="23" max="23" width="10.140625" customWidth="1"/>
-    <col min="29" max="29" width="12" bestFit="1" customWidth="1"/>
-    <col min="30" max="35" width="12.42578125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="11.85546875" customWidth="1"/>
+    <col min="29" max="29" width="12.5703125" customWidth="1"/>
+    <col min="30" max="30" width="15.42578125" style="1" customWidth="1"/>
+    <col min="31" max="35" width="12.42578125" style="1" customWidth="1"/>
     <col min="36" max="38" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="W1" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="50"/>
+      <c r="AB1" s="50"/>
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="50"/>
+      <c r="AE1" s="50"/>
+      <c r="AF1" s="50"/>
+      <c r="AG1" s="51"/>
+    </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="AB2" t="s">
+      <c r="W2" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y2" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2" s="53"/>
+      <c r="AA2" s="43"/>
+      <c r="AB2" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AC2" s="43"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="44"/>
+      <c r="AF2" s="44" t="s">
         <v>61</v>
       </c>
+      <c r="AG2" s="45"/>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
@@ -807,26 +1020,30 @@
       <c r="Q3" s="5">
         <v>13</v>
       </c>
-      <c r="Y3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC3" s="1" t="s">
+      <c r="W3" s="58">
+        <f xml:space="preserve"> 0.1450377/1000</f>
+        <v>1.4503769999999998E-4</v>
+      </c>
+      <c r="X3" s="59">
+        <v>1E-3</v>
+      </c>
+      <c r="Y3" s="59">
+        <v>3.7854099999999999E-3</v>
+      </c>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="43"/>
+      <c r="AB3" s="43"/>
+      <c r="AC3" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="AF3" s="1">
+      <c r="AD3" s="44"/>
+      <c r="AE3" s="44"/>
+      <c r="AF3" s="44">
         <v>0.55300000000000005</v>
       </c>
+      <c r="AG3" s="45"/>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>999.7</v>
-      </c>
-      <c r="C4">
-        <v>1E-3</v>
-      </c>
       <c r="D4" s="2" t="s">
         <v>32</v>
       </c>
@@ -834,66 +1051,75 @@
         <v>0</v>
       </c>
       <c r="F4" s="5">
-        <f>F3*$C$4</f>
+        <f>F3*$X$3</f>
         <v>2E-3</v>
       </c>
       <c r="G4" s="5">
-        <f t="shared" ref="G4:Q4" si="0">G3*$C$4</f>
+        <f>G3*$X$3</f>
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H4" s="5">
-        <f t="shared" si="0"/>
+        <f>H3*$X$3</f>
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="I4" s="5">
-        <f t="shared" si="0"/>
+        <f>I3*$X$3</f>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="J4" s="5">
-        <f t="shared" si="0"/>
+        <f>J3*$X$3</f>
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="K4" s="5">
-        <f t="shared" si="0"/>
+        <f>K3*$X$3</f>
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="L4" s="5">
-        <f t="shared" si="0"/>
+        <f>L3*$X$3</f>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="M4" s="5">
-        <f t="shared" si="0"/>
+        <f>M3*$X$3</f>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="N4" s="5">
-        <f t="shared" si="0"/>
+        <f>N3*$X$3</f>
         <v>0.01</v>
       </c>
       <c r="O4" s="5">
-        <f t="shared" si="0"/>
+        <f>O3*$X$3</f>
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="P4" s="5">
-        <f t="shared" si="0"/>
+        <f>P3*$X$3</f>
         <v>1.2E-2</v>
       </c>
       <c r="Q4" s="5">
-        <f t="shared" si="0"/>
+        <f>Q3*$X$3</f>
         <v>1.3000000000000001E-2</v>
       </c>
-      <c r="Y4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="21">
-        <v>2.2626E-5</v>
-      </c>
-      <c r="AB4" t="s">
+      <c r="W4" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="X4" s="63"/>
+      <c r="Y4" s="64" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z4" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA4" s="43"/>
+      <c r="AB4" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="AC4" s="1">
+      <c r="AC4" s="44">
         <f>Pintle_Area/12</f>
         <v>1.8855E-6</v>
       </c>
+      <c r="AD4" s="44"/>
+      <c r="AE4" s="44"/>
+      <c r="AF4" s="44"/>
+      <c r="AG4" s="45"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="D5" s="16" t="s">
@@ -903,74 +1129,81 @@
         <v>0</v>
       </c>
       <c r="F5" s="18">
-        <f t="shared" ref="F5:Q5" si="1">F4*$B$4</f>
+        <f>F4*$X$5</f>
         <v>1.9994000000000001</v>
       </c>
       <c r="G5" s="18">
-        <f t="shared" si="1"/>
+        <f>G4*$X$5</f>
         <v>2.9991000000000003</v>
       </c>
       <c r="H5" s="18">
-        <f t="shared" si="1"/>
+        <f>H4*$X$5</f>
         <v>3.9988000000000001</v>
       </c>
       <c r="I5" s="18">
-        <f t="shared" si="1"/>
+        <f>I4*$X$5</f>
         <v>4.9984999999999999</v>
       </c>
       <c r="J5" s="18">
-        <f t="shared" si="1"/>
+        <f>J4*$X$5</f>
         <v>5.9982000000000006</v>
       </c>
       <c r="K5" s="18">
-        <f t="shared" si="1"/>
+        <f>K4*$X$5</f>
         <v>6.9979000000000005</v>
       </c>
       <c r="L5" s="18">
-        <f t="shared" si="1"/>
+        <f>L4*$X$5</f>
         <v>7.9976000000000003</v>
       </c>
       <c r="M5" s="18">
-        <f t="shared" si="1"/>
+        <f>M4*$X$5</f>
         <v>8.997300000000001</v>
       </c>
       <c r="N5" s="18">
-        <f t="shared" si="1"/>
+        <f>N4*$X$5</f>
         <v>9.9969999999999999</v>
       </c>
       <c r="O5" s="18">
-        <f t="shared" si="1"/>
+        <f>O4*$X$5</f>
         <v>10.996700000000001</v>
       </c>
       <c r="P5" s="18">
-        <f t="shared" si="1"/>
+        <f>P4*$X$5</f>
         <v>11.996400000000001</v>
       </c>
       <c r="Q5" s="18">
-        <f t="shared" si="1"/>
+        <f>Q4*$X$5</f>
         <v>12.996100000000002</v>
       </c>
       <c r="R5" s="10"/>
-      <c r="Y5" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="21">
-        <v>2.152788E-5</v>
-      </c>
-      <c r="AC5" t="s">
+      <c r="W5" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="X5" s="44">
+        <v>999.7</v>
+      </c>
+      <c r="Y5" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="55">
+        <v>2.2626E-5</v>
+      </c>
+      <c r="AA5" s="43"/>
+      <c r="AB5" s="43"/>
+      <c r="AC5" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AD5" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="AE5" s="1" t="s">
+      <c r="AE5" s="44" t="s">
         <v>58</v>
       </c>
+      <c r="AF5" s="44"/>
+      <c r="AG5" s="45"/>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>36</v>
-      </c>
       <c r="D6" s="3" t="s">
         <v>23</v>
       </c>
@@ -1016,27 +1249,36 @@
       <c r="R6" s="12">
         <v>3.5</v>
       </c>
-      <c r="W6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB6" t="s">
+      <c r="W6" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="X6" s="44">
+        <v>1141</v>
+      </c>
+      <c r="Y6" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="55">
+        <v>2.152788E-5</v>
+      </c>
+      <c r="AA6" s="43"/>
+      <c r="AB6" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="AC6">
+      <c r="AC6" s="43">
         <v>6.8579999999999997E-4</v>
       </c>
-      <c r="AD6" s="1">
+      <c r="AD6" s="44">
         <v>1.5494E-3</v>
       </c>
-      <c r="AE6" s="1">
+      <c r="AE6" s="44">
         <f>AD6*AC6</f>
         <v>1.06257852E-6</v>
       </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>3.7854099999999999E-3</v>
-      </c>
+      <c r="AF6" s="44"/>
+      <c r="AG6" s="45"/>
+    </row>
+    <row r="7" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="3" t="s">
         <v>32</v>
       </c>
@@ -1044,61 +1286,72 @@
         <v>0</v>
       </c>
       <c r="F7" s="11">
-        <f>F6*$C$7</f>
+        <f>F6*$Y$3</f>
         <v>1.892705E-3</v>
       </c>
       <c r="G7" s="11">
-        <f t="shared" ref="G7:R7" si="2">G6*$C$7</f>
+        <f>G6*$Y$3</f>
         <v>2.8390575E-3</v>
       </c>
       <c r="H7" s="11">
-        <f t="shared" si="2"/>
+        <f>H6*$Y$3</f>
         <v>3.7854099999999999E-3</v>
       </c>
       <c r="I7" s="11">
-        <f t="shared" si="2"/>
+        <f>I6*$Y$3</f>
         <v>4.7317625000000002E-3</v>
       </c>
       <c r="J7" s="11">
-        <f t="shared" si="2"/>
+        <f>J6*$Y$3</f>
         <v>5.6781150000000001E-3</v>
       </c>
       <c r="K7" s="11">
-        <f t="shared" si="2"/>
+        <f>K6*$Y$3</f>
         <v>6.6244674999999999E-3</v>
       </c>
       <c r="L7" s="11">
-        <f t="shared" si="2"/>
+        <f>L6*$Y$3</f>
         <v>7.5708199999999998E-3</v>
       </c>
       <c r="M7" s="11">
-        <f t="shared" si="2"/>
+        <f>M6*$Y$3</f>
         <v>8.5171724999999997E-3</v>
       </c>
       <c r="N7" s="11">
-        <f t="shared" si="2"/>
+        <f>N6*$Y$3</f>
         <v>9.4635250000000004E-3</v>
       </c>
       <c r="O7" s="11">
-        <f t="shared" si="2"/>
+        <f>O6*$Y$3</f>
         <v>1.0409877499999999E-2</v>
       </c>
       <c r="P7" s="11">
-        <f t="shared" si="2"/>
+        <f>P6*$Y$3</f>
         <v>1.135623E-2</v>
       </c>
       <c r="Q7" s="11">
-        <f t="shared" si="2"/>
+        <f>Q6*$Y$3</f>
         <v>1.2302582499999999E-2</v>
       </c>
       <c r="R7" s="11">
-        <f t="shared" si="2"/>
+        <f>R6*$Y$3</f>
         <v>1.3248935E-2</v>
       </c>
-      <c r="W7" s="8">
-        <f xml:space="preserve"> 0.1450377/1000</f>
-        <v>1.4503769999999998E-4</v>
-      </c>
+      <c r="W7" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="X7" s="47">
+        <v>877.8</v>
+      </c>
+      <c r="Y7" s="57"/>
+      <c r="Z7" s="57"/>
+      <c r="AA7" s="46"/>
+      <c r="AB7" s="46"/>
+      <c r="AC7" s="46"/>
+      <c r="AD7" s="47"/>
+      <c r="AE7" s="47"/>
+      <c r="AF7" s="47"/>
+      <c r="AG7" s="48"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="D8" s="13" t="s">
@@ -1108,55 +1361,55 @@
         <v>0</v>
       </c>
       <c r="F8" s="15">
-        <f>F7*$B$4</f>
+        <f>F7*$X$5</f>
         <v>1.8921371885</v>
       </c>
       <c r="G8" s="15">
-        <f t="shared" ref="G8:R8" si="3">G7*$B$4</f>
+        <f>G7*$X$5</f>
         <v>2.8382057827500002</v>
       </c>
       <c r="H8" s="15">
-        <f t="shared" si="3"/>
+        <f>H7*$X$5</f>
         <v>3.784274377</v>
       </c>
       <c r="I8" s="15">
-        <f t="shared" si="3"/>
+        <f>I7*$X$5</f>
         <v>4.7303429712500007</v>
       </c>
       <c r="J8" s="15">
-        <f t="shared" si="3"/>
+        <f>J7*$X$5</f>
         <v>5.6764115655000005</v>
       </c>
       <c r="K8" s="15">
-        <f t="shared" si="3"/>
+        <f>K7*$X$5</f>
         <v>6.6224801597500003</v>
       </c>
       <c r="L8" s="15">
-        <f t="shared" si="3"/>
+        <f>L7*$X$5</f>
         <v>7.568548754</v>
       </c>
       <c r="M8" s="15">
-        <f t="shared" si="3"/>
+        <f>M7*$X$5</f>
         <v>8.5146173482500007</v>
       </c>
       <c r="N8" s="15">
-        <f t="shared" si="3"/>
+        <f>N7*$X$5</f>
         <v>9.4606859425000014</v>
       </c>
       <c r="O8" s="15">
-        <f t="shared" si="3"/>
+        <f>O7*$X$5</f>
         <v>10.40675453675</v>
       </c>
       <c r="P8" s="15">
-        <f t="shared" si="3"/>
+        <f>P7*$X$5</f>
         <v>11.352823131000001</v>
       </c>
       <c r="Q8" s="15">
-        <f t="shared" si="3"/>
+        <f>Q7*$X$5</f>
         <v>12.29889172525</v>
       </c>
       <c r="R8" s="15">
-        <f t="shared" si="3"/>
+        <f>R7*$X$5</f>
         <v>13.244960319500001</v>
       </c>
     </row>
@@ -1182,13 +1435,13 @@
         <v>38</v>
       </c>
       <c r="V9" s="35"/>
-      <c r="W9" s="23" t="s">
+      <c r="W9" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="X9" s="23" t="s">
+      <c r="X9" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="Z9" s="23"/>
+      <c r="Z9" s="22"/>
       <c r="AD9" s="9"/>
       <c r="AE9" s="9"/>
       <c r="AF9" s="9"/>
@@ -1259,13 +1512,13 @@
       <c r="P11" s="34"/>
       <c r="Q11" s="34"/>
       <c r="R11" s="34"/>
-      <c r="T11" s="26" t="s">
+      <c r="T11" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="U11" s="26"/>
-      <c r="V11" s="26"/>
-      <c r="W11" s="26"/>
-      <c r="X11" s="26"/>
+      <c r="U11" s="25"/>
+      <c r="V11" s="25"/>
+      <c r="W11" s="25"/>
+      <c r="X11" s="25"/>
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
@@ -1319,10 +1572,10 @@
         <v>16.100000000000001</v>
       </c>
       <c r="V12" s="1">
-        <f>U12/$W$7</f>
+        <f>U12/$W$3</f>
         <v>111005.62129708347</v>
       </c>
-      <c r="W12" s="22">
+      <c r="W12" s="21">
         <f>T12/(Density_h20*Annulus_area)</f>
         <v>12.538970961846575</v>
       </c>
@@ -1382,10 +1635,10 @@
         <v>19.2</v>
       </c>
       <c r="V13" s="1">
-        <f>U13/$W$7</f>
+        <f>U13/$W$3</f>
         <v>132379.37446608712</v>
       </c>
-      <c r="W13" s="22">
+      <c r="W13" s="21">
         <f>T13/(Density_h20*Annulus_area)</f>
         <v>14.386053592920568</v>
       </c>
@@ -1445,10 +1698,10 @@
         <v>18.899999999999999</v>
       </c>
       <c r="V14" s="1">
-        <f>U14/$W$7</f>
+        <f>U14/$W$3</f>
         <v>130310.94674005448</v>
       </c>
-      <c r="W14" s="22">
+      <c r="W14" s="21">
         <f>T14/(Density_h20*Annulus_area)</f>
         <v>14.514121204572028</v>
       </c>
@@ -1459,17 +1712,17 @@
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
-      <c r="T15" s="25" t="s">
+      <c r="T15" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="U15" s="25"/>
-      <c r="V15" s="25"/>
-      <c r="W15" s="25"/>
-      <c r="X15" s="25"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="24"/>
+      <c r="W15" s="24"/>
+      <c r="X15" s="24"/>
       <c r="Y15" t="s">
         <v>49</v>
       </c>
-      <c r="Z15" s="27">
+      <c r="Z15" s="26">
         <f>AVERAGE(X12:X18)</f>
         <v>1.3004532412336933</v>
       </c>
@@ -1525,10 +1778,10 @@
         <v>25.9</v>
       </c>
       <c r="V16" s="1">
-        <f>U16/$W$7</f>
+        <f>U16/$W$3</f>
         <v>178574.26034748208</v>
       </c>
-      <c r="W16" s="22">
+      <c r="W16" s="21">
         <f>T16/(Density_h20*Annulus_area)</f>
         <v>15.823017845505417</v>
       </c>
@@ -1588,10 +1841,10 @@
         <v>23.9</v>
       </c>
       <c r="V17" s="1">
-        <f>U17/$W$7</f>
+        <f>U17/$W$3</f>
         <v>164784.74217393133</v>
       </c>
-      <c r="W17" s="22">
+      <c r="W17" s="21">
         <f>T17/(Density_h20*Annulus_area)</f>
         <v>15.627142696479785</v>
       </c>
@@ -1651,10 +1904,10 @@
         <v>16.2</v>
       </c>
       <c r="V18" s="1">
-        <f>U18/$W$7</f>
+        <f>U18/$W$3</f>
         <v>111695.09720576099</v>
       </c>
-      <c r="W18" s="22">
+      <c r="W18" s="21">
         <f>T18/(Density_h20*Annulus_area)</f>
         <v>14.277774941828433</v>
       </c>
@@ -1665,13 +1918,13 @@
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
-      <c r="T19" s="25" t="s">
+      <c r="T19" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="U19" s="25"/>
-      <c r="V19" s="25"/>
-      <c r="W19" s="25"/>
-      <c r="X19" s="25"/>
+      <c r="U19" s="24"/>
+      <c r="V19" s="24"/>
+      <c r="W19" s="24"/>
+      <c r="X19" s="24"/>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1724,7 +1977,7 @@
         <v>14.1</v>
       </c>
       <c r="V20" s="1">
-        <f>U20/$W$7</f>
+        <f>U20/$W$3</f>
         <v>97216.103123532725</v>
       </c>
       <c r="W20">
@@ -1793,7 +2046,7 @@
         <v>12.6</v>
       </c>
       <c r="V21" s="1">
-        <f>U21/$W$7</f>
+        <f>U21/$W$3</f>
         <v>86873.964493369669</v>
       </c>
       <c r="W21">
@@ -1862,7 +2115,7 @@
         <v>16.899999999999999</v>
       </c>
       <c r="V22" s="1">
-        <f>U22/$W$7</f>
+        <f>U22/$W$3</f>
         <v>116521.42856650375</v>
       </c>
       <c r="W22">
@@ -1876,17 +2129,17 @@
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
-      <c r="T23" s="25" t="s">
+      <c r="T23" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="U23" s="25"/>
-      <c r="V23" s="25"/>
-      <c r="W23" s="25"/>
-      <c r="X23" s="25"/>
+      <c r="U23" s="24"/>
+      <c r="V23" s="24"/>
+      <c r="W23" s="24"/>
+      <c r="X23" s="24"/>
       <c r="Y23" t="s">
         <v>50</v>
       </c>
-      <c r="Z23" s="27">
+      <c r="Z23" s="26">
         <f>AVERAGE(X20:X27)</f>
         <v>2.5145416329988741</v>
       </c>
@@ -1948,7 +2201,7 @@
         <v>36.6</v>
       </c>
       <c r="V24" s="1">
-        <f>U24/$W$7</f>
+        <f>U24/$W$3</f>
         <v>252348.18257597857</v>
       </c>
       <c r="W24">
@@ -1959,7 +2212,7 @@
         <f>(2*V24)/(Density_h20*W24^2)</f>
         <v>2.6114485915684851</v>
       </c>
-      <c r="Y24" s="22"/>
+      <c r="Y24" s="21"/>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -2018,7 +2271,7 @@
         <v>36.9</v>
       </c>
       <c r="V25" s="1">
-        <f>U25/$W$7</f>
+        <f>U25/$W$3</f>
         <v>254416.61030201116</v>
       </c>
       <c r="W25">
@@ -2029,7 +2282,7 @@
         <f>(2*V25)/(Density_h20*W25^2)</f>
         <v>2.5208035831069133</v>
       </c>
-      <c r="Y25" s="22"/>
+      <c r="Y25" s="21"/>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -2088,7 +2341,7 @@
         <v>36.9</v>
       </c>
       <c r="V26" s="1">
-        <f>U26/$W$7</f>
+        <f>U26/$W$3</f>
         <v>254416.61030201116</v>
       </c>
       <c r="W26">
@@ -2099,7 +2352,7 @@
         <f>(2*V26)/(Density_h20*W26^2)</f>
         <v>2.5761143009166725</v>
       </c>
-      <c r="Y26" s="22"/>
+      <c r="Y26" s="21"/>
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -2158,7 +2411,7 @@
         <v>36.9</v>
       </c>
       <c r="V27" s="1">
-        <f>U27/$W$7</f>
+        <f>U27/$W$3</f>
         <v>254416.61030201116</v>
       </c>
       <c r="W27">
@@ -2169,7 +2422,7 @@
         <f>(2*V27)/(Density_h20*W27^2)</f>
         <v>2.6443495539368849</v>
       </c>
-      <c r="Y27" s="22"/>
+      <c r="Y27" s="21"/>
       <c r="AD27" s="33" t="s">
         <v>62</v>
       </c>
@@ -2203,54 +2456,54 @@
       <c r="O28" s="9"/>
       <c r="P28" s="9"/>
       <c r="T28" s="19"/>
-      <c r="U28" s="1" t="s">
+      <c r="U28" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="V28" s="1" t="s">
+      <c r="V28" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="W28" s="1" t="s">
+      <c r="W28" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="X28" s="1" t="s">
+      <c r="X28" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="Y28" s="1" t="s">
+      <c r="Y28" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="Z28" s="1" t="s">
+      <c r="Z28" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="AA28" s="1" t="s">
+      <c r="AA28" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="AB28" s="1" t="s">
+      <c r="AB28" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="AC28" s="1" t="s">
+      <c r="AC28" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AD28" s="24" t="s">
+      <c r="AD28" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="AE28" s="24" t="s">
+      <c r="AE28" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="AF28" s="24" t="s">
+      <c r="AF28" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="AG28" s="24" t="s">
+      <c r="AG28" s="7" t="s">
         <v>67</v>
       </c>
       <c r="AH28"/>
       <c r="AI28"/>
-      <c r="AK28" s="24" t="s">
+      <c r="AK28" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="AL28" s="24" t="s">
+      <c r="AL28" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="AM28" s="24" t="s">
+      <c r="AM28" s="23" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2258,52 +2511,52 @@
       <c r="C29" s="1"/>
       <c r="E29" s="9"/>
       <c r="T29" s="19"/>
-      <c r="U29" s="1" t="s">
+      <c r="U29" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="V29" s="1" t="s">
+      <c r="V29" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="W29" s="1" t="s">
+      <c r="W29" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="X29" s="1" t="s">
+      <c r="X29" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="Y29" s="1" t="s">
+      <c r="Y29" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="Z29" s="1" t="s">
+      <c r="Z29" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="AA29" s="1" t="s">
+      <c r="AA29" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="AB29" s="1" t="s">
+      <c r="AB29" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="AC29" s="1" t="s">
+      <c r="AC29" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="AD29" s="24" t="s">
+      <c r="AD29" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="AE29" s="24" t="s">
+      <c r="AE29" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="AF29" s="24" t="s">
+      <c r="AF29" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AG29"/>
+      <c r="AG29" s="6"/>
       <c r="AH29"/>
       <c r="AI29"/>
-      <c r="AK29" s="24" t="s">
+      <c r="AK29" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="AL29" s="24" t="s">
+      <c r="AL29" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="AM29" s="24" t="s">
+      <c r="AM29" s="23" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2344,54 +2597,54 @@
         <f>SLOPE(E8:R8,E30:R30)</f>
         <v>0.46802132631680521</v>
       </c>
-      <c r="U30" s="1">
+      <c r="U30" s="36">
         <v>26.2</v>
       </c>
-      <c r="V30" s="1">
+      <c r="V30" s="32">
         <v>6.3</v>
       </c>
-      <c r="W30" s="1">
-        <f t="shared" ref="W30:X32" si="4">U30/$W$7</f>
+      <c r="W30" s="36">
+        <f>U30/$W$3</f>
         <v>180642.6880735147</v>
       </c>
-      <c r="X30" s="1">
-        <f t="shared" si="4"/>
+      <c r="X30" s="32">
+        <f>V30/$W$3</f>
         <v>43436.982246684835</v>
       </c>
-      <c r="Y30" s="22">
-        <f t="shared" ref="Y30:Y38" si="5">SQRT((2*W30)/(kl_annulus*Density_h20))</f>
+      <c r="Y30" s="37">
+        <f t="shared" ref="Y30:Y38" si="0">SQRT((2*W30)/(kl_annulus*Density_h20))</f>
         <v>16.670283078667804</v>
       </c>
-      <c r="Z30" s="22">
-        <f t="shared" ref="Z30:Z38" si="6">SQRT((2*X30)/(kl_pintle*Density_h20))</f>
+      <c r="Z30" s="40">
+        <f t="shared" ref="Z30:Z38" si="1">SQRT((2*X30)/(kl_pintle*Density_h20))</f>
         <v>5.8786899991591568</v>
       </c>
-      <c r="AA30" s="19">
-        <f t="shared" ref="AA30:AA38" si="7">Y30*Density_h20*Annulus_area</f>
+      <c r="AA30" s="38">
+        <f t="shared" ref="AA30:AA38" si="2">Y30*Density_h20*Annulus_area</f>
         <v>0.35876819092748596</v>
       </c>
-      <c r="AB30" s="19">
-        <f t="shared" ref="AB30:AB38" si="8">Z30*Density_h20*Pintle_Area</f>
+      <c r="AB30" s="41">
+        <f t="shared" ref="AB30:AB38" si="3">Z30*Density_h20*Pintle_Area</f>
         <v>0.13297133654899879</v>
       </c>
-      <c r="AC30" s="19">
-        <f t="shared" ref="AC30:AC38" si="9">AB30+AA30</f>
+      <c r="AC30" s="42">
+        <f t="shared" ref="AC30:AC38" si="4">AB30+AA30</f>
         <v>0.49173952747648475</v>
       </c>
-      <c r="AD30">
-        <f t="shared" ref="AD30:AD38" si="10">(blockage_factor*AA30)*Y30</f>
+      <c r="AD30" s="39">
+        <f t="shared" ref="AD30:AD38" si="5">(blockage_factor*AA30)*Y30</f>
         <v>3.3073643182176498</v>
       </c>
-      <c r="AE30">
-        <f t="shared" ref="AE30:AE38" si="11">AB30*Z30</f>
+      <c r="AE30" s="3">
+        <f t="shared" ref="AE30:AE38" si="6">AB30*Z30</f>
         <v>0.78169726634542558</v>
       </c>
-      <c r="AF30">
-        <f t="shared" ref="AF30:AF38" si="12">AD30/AE30</f>
+      <c r="AF30" s="2">
+        <f t="shared" ref="AF30:AF38" si="7">AD30/AE30</f>
         <v>4.2310040735848666</v>
       </c>
-      <c r="AG30">
-        <f t="shared" ref="AG30:AG38" si="13">ATAN(AE30/AD30)*180/PI()</f>
+      <c r="AG30" s="6">
+        <f t="shared" ref="AG30:AG38" si="8">ATAN(AE30/AD30)*180/PI()</f>
         <v>13.297858414298471</v>
       </c>
       <c r="AJ30" s="1"/>
@@ -2461,61 +2714,55 @@
         <f>SLOPE($E$8:$P$8,E31:P31)</f>
         <v>0.52215563380049257</v>
       </c>
-      <c r="U31" s="1">
+      <c r="U31" s="36">
         <v>34</v>
       </c>
-      <c r="V31" s="1">
+      <c r="V31" s="32">
         <v>6.1</v>
       </c>
-      <c r="W31" s="1">
+      <c r="W31" s="36">
+        <f>U31/$W$3</f>
+        <v>234421.80895036258</v>
+      </c>
+      <c r="X31" s="32">
+        <f>V31/$W$3</f>
+        <v>42058.030429329759</v>
+      </c>
+      <c r="Y31" s="37">
+        <f t="shared" si="0"/>
+        <v>18.990298336054028</v>
+      </c>
+      <c r="Z31" s="40">
+        <f t="shared" si="1"/>
+        <v>5.7846248900611554</v>
+      </c>
+      <c r="AA31" s="38">
+        <f t="shared" si="2"/>
+        <v>0.40869821748364793</v>
+      </c>
+      <c r="AB31" s="41">
+        <f t="shared" si="3"/>
+        <v>0.13084365788569496</v>
+      </c>
+      <c r="AC31" s="42">
         <f t="shared" si="4"/>
-        <v>234421.80895036258</v>
-      </c>
-      <c r="X31" s="1">
-        <f t="shared" si="4"/>
-        <v>42058.030429329759</v>
-      </c>
-      <c r="Y31" s="22">
+        <v>0.53954187536934284</v>
+      </c>
+      <c r="AD31" s="39">
         <f t="shared" si="5"/>
-        <v>18.990298336054028</v>
-      </c>
-      <c r="Z31" s="22">
+        <v>4.2919994969236663</v>
+      </c>
+      <c r="AE31" s="3">
         <f t="shared" si="6"/>
-        <v>5.7846248900611554</v>
-      </c>
-      <c r="AA31" s="19">
+        <v>0.75688148011223766</v>
+      </c>
+      <c r="AF31" s="2">
         <f t="shared" si="7"/>
-        <v>0.40869821748364793</v>
-      </c>
-      <c r="AB31" s="19">
+        <v>5.6706361692020888</v>
+      </c>
+      <c r="AG31" s="6">
         <f t="shared" si="8"/>
-        <v>0.13084365788569496</v>
-      </c>
-      <c r="AC31" s="19">
-        <f t="shared" si="9"/>
-        <v>0.53954187536934284</v>
-      </c>
-      <c r="AD31">
-        <f t="shared" si="10"/>
-        <v>4.2919994969236663</v>
-      </c>
-      <c r="AE31">
-        <f t="shared" si="11"/>
-        <v>0.75688148011223766</v>
-      </c>
-      <c r="AF31">
-        <f t="shared" si="12"/>
-        <v>5.6706361692020888</v>
-      </c>
-      <c r="AG31">
-        <f t="shared" si="13"/>
         <v>10.001115599938339</v>
-      </c>
-      <c r="AH31" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI31" s="1">
-        <v>1141</v>
       </c>
       <c r="AJ31" s="1"/>
       <c r="AK31">
@@ -2584,61 +2831,55 @@
         <f>SLOPE($E$8:$P$8,E32:P32)</f>
         <v>0.48401389007890933</v>
       </c>
-      <c r="U32" s="1">
+      <c r="U32" s="36">
         <v>28.6</v>
       </c>
-      <c r="V32" s="1">
+      <c r="V32" s="32">
         <v>4.9000000000000004</v>
       </c>
-      <c r="W32" s="1">
+      <c r="W32" s="36">
+        <f>U32/$W$3</f>
+        <v>197190.1098817756</v>
+      </c>
+      <c r="X32" s="32">
+        <f>V32/$W$3</f>
+        <v>33784.319525199317</v>
+      </c>
+      <c r="Y32" s="37">
+        <f t="shared" si="0"/>
+        <v>17.417079956789561</v>
+      </c>
+      <c r="Z32" s="40">
+        <f t="shared" si="1"/>
+        <v>5.1845172575392118</v>
+      </c>
+      <c r="AA32" s="38">
+        <f t="shared" si="2"/>
+        <v>0.37484032141799278</v>
+      </c>
+      <c r="AB32" s="41">
+        <f t="shared" si="3"/>
+        <v>0.11726969600284147</v>
+      </c>
+      <c r="AC32" s="42">
         <f t="shared" si="4"/>
-        <v>197190.1098817756</v>
-      </c>
-      <c r="X32" s="1">
-        <f t="shared" si="4"/>
-        <v>33784.319525199317</v>
-      </c>
-      <c r="Y32" s="22">
+        <v>0.49211001742083427</v>
+      </c>
+      <c r="AD32" s="39">
         <f t="shared" si="5"/>
-        <v>17.417079956789561</v>
-      </c>
-      <c r="Z32" s="22">
+        <v>3.6103289885887313</v>
+      </c>
+      <c r="AE32" s="3">
         <f t="shared" si="6"/>
-        <v>5.1845172575392118</v>
-      </c>
-      <c r="AA32" s="19">
+        <v>0.6079867627131087</v>
+      </c>
+      <c r="AF32" s="2">
         <f t="shared" si="7"/>
-        <v>0.37484032141799278</v>
-      </c>
-      <c r="AB32" s="19">
+        <v>5.9381703846278322</v>
+      </c>
+      <c r="AG32" s="6">
         <f t="shared" si="8"/>
-        <v>0.11726969600284147</v>
-      </c>
-      <c r="AC32" s="19">
-        <f t="shared" si="9"/>
-        <v>0.49211001742083427</v>
-      </c>
-      <c r="AD32">
-        <f t="shared" si="10"/>
-        <v>3.6103289885887313</v>
-      </c>
-      <c r="AE32">
-        <f t="shared" si="11"/>
-        <v>0.6079867627131087</v>
-      </c>
-      <c r="AF32">
-        <f t="shared" si="12"/>
-        <v>5.9381703846278322</v>
-      </c>
-      <c r="AG32">
-        <f t="shared" si="13"/>
         <v>9.5590371193691137</v>
-      </c>
-      <c r="AH32" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI32" s="1">
-        <v>877.8</v>
       </c>
       <c r="AJ32" s="1"/>
       <c r="AK32">
@@ -2668,54 +2909,54 @@
         <v>28</v>
       </c>
       <c r="E33" s="9"/>
-      <c r="U33" s="24">
+      <c r="U33" s="36">
         <v>36.6</v>
       </c>
-      <c r="V33" s="24">
+      <c r="V33" s="32">
         <v>16.57</v>
       </c>
-      <c r="W33" s="24">
-        <f t="shared" ref="W33:W34" si="14">U33/$W$7</f>
+      <c r="W33" s="36">
+        <f>U33/$W$3</f>
         <v>252348.18257597857</v>
       </c>
-      <c r="X33" s="24">
-        <f t="shared" ref="X33:X34" si="15">V33/$W$7</f>
+      <c r="X33" s="32">
+        <f>V33/$W$3</f>
         <v>114246.15806786789</v>
       </c>
-      <c r="Y33" s="22">
+      <c r="Y33" s="37">
+        <f t="shared" si="0"/>
+        <v>19.703023335234857</v>
+      </c>
+      <c r="Z33" s="40">
+        <f t="shared" si="1"/>
+        <v>9.5339207734425813</v>
+      </c>
+      <c r="AA33" s="38">
+        <f t="shared" si="2"/>
+        <v>0.42403707270153634</v>
+      </c>
+      <c r="AB33" s="41">
+        <f t="shared" si="3"/>
+        <v>0.21564977707248589</v>
+      </c>
+      <c r="AC33" s="42">
+        <f t="shared" si="4"/>
+        <v>0.63968684977402224</v>
+      </c>
+      <c r="AD33" s="39">
         <f t="shared" si="5"/>
-        <v>19.703023335234857</v>
-      </c>
-      <c r="Z33" s="22">
+        <v>4.6202112231590071</v>
+      </c>
+      <c r="AE33" s="3">
         <f t="shared" si="6"/>
-        <v>9.5339207734425813</v>
-      </c>
-      <c r="AA33" s="19">
+        <v>2.0559878894196348</v>
+      </c>
+      <c r="AF33" s="2">
         <f t="shared" si="7"/>
-        <v>0.42403707270153634</v>
-      </c>
-      <c r="AB33" s="19">
+        <v>2.2471976838653474</v>
+      </c>
+      <c r="AG33" s="6">
         <f t="shared" si="8"/>
-        <v>0.21564977707248589</v>
-      </c>
-      <c r="AC33" s="19">
-        <f t="shared" si="9"/>
-        <v>0.63968684977402224</v>
-      </c>
-      <c r="AD33">
-        <f t="shared" si="10"/>
-        <v>4.6202112231590071</v>
-      </c>
-      <c r="AE33">
-        <f t="shared" si="11"/>
-        <v>2.0559878894196348</v>
-      </c>
-      <c r="AF33">
-        <f t="shared" si="12"/>
-        <v>2.2471976838653474</v>
-      </c>
-      <c r="AG33">
-        <f t="shared" si="13"/>
         <v>23.989000816009955</v>
       </c>
       <c r="AH33"/>
@@ -2734,108 +2975,108 @@
       <c r="D34" t="s">
         <v>28</v>
       </c>
-      <c r="U34" s="24">
+      <c r="U34" s="36">
         <v>30.59</v>
       </c>
-      <c r="V34" s="24">
+      <c r="V34" s="32">
         <v>11.49</v>
       </c>
-      <c r="W34" s="24">
-        <f t="shared" si="14"/>
+      <c r="W34" s="36">
+        <f>U34/$W$3</f>
         <v>210910.68046445856</v>
       </c>
-      <c r="X34" s="24">
-        <f t="shared" si="15"/>
+      <c r="X34" s="32">
+        <f>V34/$W$3</f>
         <v>79220.781907049008</v>
       </c>
-      <c r="Y34" s="22">
+      <c r="Y34" s="37">
+        <f t="shared" si="0"/>
+        <v>18.012834861153678</v>
+      </c>
+      <c r="Z34" s="40">
+        <f t="shared" si="1"/>
+        <v>7.9390822033664019</v>
+      </c>
+      <c r="AA34" s="38">
+        <f t="shared" si="2"/>
+        <v>0.38766181390652787</v>
+      </c>
+      <c r="AB34" s="41">
+        <f t="shared" si="3"/>
+        <v>0.17957578503118821</v>
+      </c>
+      <c r="AC34" s="42">
+        <f t="shared" si="4"/>
+        <v>0.56723759893771608</v>
+      </c>
+      <c r="AD34" s="39">
         <f t="shared" si="5"/>
-        <v>18.012834861153678</v>
-      </c>
-      <c r="Z34" s="22">
+        <v>3.8615371944380872</v>
+      </c>
+      <c r="AE34" s="3">
         <f t="shared" si="6"/>
-        <v>7.9390822033664019</v>
-      </c>
-      <c r="AA34" s="19">
+        <v>1.4256669190966571</v>
+      </c>
+      <c r="AF34" s="2">
         <f t="shared" si="7"/>
-        <v>0.38766181390652787</v>
-      </c>
-      <c r="AB34" s="19">
+        <v>2.7085830096169072</v>
+      </c>
+      <c r="AG34" s="6">
         <f t="shared" si="8"/>
-        <v>0.17957578503118821</v>
-      </c>
-      <c r="AC34" s="19">
-        <f t="shared" si="9"/>
-        <v>0.56723759893771608</v>
-      </c>
-      <c r="AD34">
-        <f t="shared" si="10"/>
-        <v>3.8615371944380872</v>
-      </c>
-      <c r="AE34">
-        <f t="shared" si="11"/>
-        <v>1.4256669190966571</v>
-      </c>
-      <c r="AF34">
-        <f t="shared" si="12"/>
-        <v>2.7085830096169072</v>
-      </c>
-      <c r="AG34">
-        <f t="shared" si="13"/>
         <v>20.263981320060967</v>
       </c>
       <c r="AH34"/>
       <c r="AI34"/>
     </row>
     <row r="35" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="U35" s="24">
+      <c r="U35" s="36">
         <v>30.4</v>
       </c>
-      <c r="V35" s="24">
+      <c r="V35" s="32">
         <v>22.125</v>
       </c>
-      <c r="W35" s="24">
-        <f t="shared" ref="W35" si="16">U35/$W$7</f>
+      <c r="W35" s="36">
+        <f>U35/$W$3</f>
         <v>209600.67623797126</v>
       </c>
-      <c r="X35" s="24">
-        <f t="shared" ref="X35" si="17">V35/$W$7</f>
+      <c r="X35" s="32">
+        <f>V35/$W$3</f>
         <v>152546.54479490506</v>
       </c>
-      <c r="Y35" s="22">
+      <c r="Y35" s="37">
+        <f t="shared" si="0"/>
+        <v>17.956807245301501</v>
+      </c>
+      <c r="Z35" s="40">
+        <f t="shared" si="1"/>
+        <v>11.016710171011155</v>
+      </c>
+      <c r="AA35" s="38">
+        <f t="shared" si="2"/>
+        <v>0.38645601996251333</v>
+      </c>
+      <c r="AB35" s="41">
+        <f t="shared" si="3"/>
+        <v>0.24918930510399961</v>
+      </c>
+      <c r="AC35" s="42">
+        <f t="shared" si="4"/>
+        <v>0.63564532506651295</v>
+      </c>
+      <c r="AD35" s="39">
         <f t="shared" si="5"/>
-        <v>17.956807245301501</v>
-      </c>
-      <c r="Z35" s="22">
+        <v>3.8375524913670427</v>
+      </c>
+      <c r="AE35" s="3">
         <f t="shared" si="6"/>
-        <v>11.016710171011155</v>
-      </c>
-      <c r="AA35" s="19">
+        <v>2.7452463520464345</v>
+      </c>
+      <c r="AF35" s="2">
         <f t="shared" si="7"/>
-        <v>0.38645601996251333</v>
-      </c>
-      <c r="AB35" s="19">
+        <v>1.3978900248811377</v>
+      </c>
+      <c r="AG35" s="6">
         <f t="shared" si="8"/>
-        <v>0.24918930510399961</v>
-      </c>
-      <c r="AC35" s="19">
-        <f t="shared" si="9"/>
-        <v>0.63564532506651295</v>
-      </c>
-      <c r="AD35">
-        <f t="shared" si="10"/>
-        <v>3.8375524913670427</v>
-      </c>
-      <c r="AE35">
-        <f t="shared" si="11"/>
-        <v>2.7452463520464345</v>
-      </c>
-      <c r="AF35">
-        <f t="shared" si="12"/>
-        <v>1.3978900248811377</v>
-      </c>
-      <c r="AG35">
-        <f t="shared" si="13"/>
         <v>35.578560702570691</v>
       </c>
       <c r="AH35"/>
@@ -2845,54 +3086,54 @@
       <c r="T36" t="s">
         <v>68</v>
       </c>
-      <c r="U36" s="24">
+      <c r="U36" s="36">
         <v>56</v>
       </c>
-      <c r="V36" s="24">
+      <c r="V36" s="32">
         <v>59</v>
       </c>
-      <c r="W36" s="24">
-        <f t="shared" ref="W36" si="18">U36/$W$7</f>
+      <c r="W36" s="36">
+        <f>U36/$W$3</f>
         <v>386106.50885942072</v>
       </c>
-      <c r="X36" s="24">
-        <f t="shared" ref="X36" si="19">V36/$W$7</f>
+      <c r="X36" s="32">
+        <f>V36/$W$3</f>
         <v>406790.78611974686</v>
       </c>
-      <c r="Y36" s="22">
+      <c r="Y36" s="37">
+        <f t="shared" si="0"/>
+        <v>24.371729119889299</v>
+      </c>
+      <c r="Z36" s="40">
+        <f t="shared" si="1"/>
+        <v>17.990212375404628</v>
+      </c>
+      <c r="AA36" s="38">
+        <f t="shared" si="2"/>
+        <v>0.52451425838751686</v>
+      </c>
+      <c r="AB36" s="41">
+        <f t="shared" si="3"/>
+        <v>0.40692443124234334</v>
+      </c>
+      <c r="AC36" s="42">
+        <f t="shared" si="4"/>
+        <v>0.93143868962986021</v>
+      </c>
+      <c r="AD36" s="39">
         <f t="shared" si="5"/>
-        <v>24.371729119889299</v>
-      </c>
-      <c r="Z36" s="22">
+        <v>7.0691756419919223</v>
+      </c>
+      <c r="AE36" s="3">
         <f t="shared" si="6"/>
-        <v>17.990212375404628</v>
-      </c>
-      <c r="AA36" s="19">
+        <v>7.3206569387904947</v>
+      </c>
+      <c r="AF36" s="2">
         <f t="shared" si="7"/>
-        <v>0.52451425838751686</v>
-      </c>
-      <c r="AB36" s="19">
+        <v>0.96564771455604892</v>
+      </c>
+      <c r="AG36" s="6">
         <f t="shared" si="8"/>
-        <v>0.40692443124234334</v>
-      </c>
-      <c r="AC36" s="19">
-        <f t="shared" si="9"/>
-        <v>0.93143868962986021</v>
-      </c>
-      <c r="AD36">
-        <f t="shared" si="10"/>
-        <v>7.0691756419919223</v>
-      </c>
-      <c r="AE36">
-        <f t="shared" si="11"/>
-        <v>7.3206569387904947</v>
-      </c>
-      <c r="AF36">
-        <f t="shared" si="12"/>
-        <v>0.96564771455604892</v>
-      </c>
-      <c r="AG36">
-        <f t="shared" si="13"/>
         <v>46.001217366435114</v>
       </c>
       <c r="AK36">
@@ -2915,54 +3156,54 @@
       <c r="T37" t="s">
         <v>68</v>
       </c>
-      <c r="U37" s="24">
+      <c r="U37" s="36">
         <v>36.6</v>
       </c>
-      <c r="V37" s="24">
+      <c r="V37" s="32">
         <v>36.6</v>
       </c>
-      <c r="W37" s="24">
-        <f t="shared" ref="W37" si="20">U37/$W$7</f>
+      <c r="W37" s="36">
+        <f>U37/$W$3</f>
         <v>252348.18257597857</v>
       </c>
-      <c r="X37" s="24">
-        <f t="shared" ref="X37" si="21">V37/$W$7</f>
+      <c r="X37" s="32">
+        <f>V37/$W$3</f>
         <v>252348.18257597857</v>
       </c>
-      <c r="Y37" s="22">
+      <c r="Y37" s="37">
+        <f t="shared" si="0"/>
+        <v>19.703023335234857</v>
+      </c>
+      <c r="Z37" s="40">
+        <f t="shared" si="1"/>
+        <v>14.169379334053069</v>
+      </c>
+      <c r="AA37" s="38">
+        <f t="shared" si="2"/>
+        <v>0.42403707270153634</v>
+      </c>
+      <c r="AB37" s="41">
+        <f t="shared" si="3"/>
+        <v>0.32050019789924106</v>
+      </c>
+      <c r="AC37" s="42">
+        <f t="shared" si="4"/>
+        <v>0.74453727060077735</v>
+      </c>
+      <c r="AD37" s="39">
         <f t="shared" si="5"/>
-        <v>19.703023335234857</v>
-      </c>
-      <c r="Z37" s="22">
+        <v>4.6202112231590071</v>
+      </c>
+      <c r="AE37" s="3">
         <f t="shared" si="6"/>
-        <v>14.169379334053069</v>
-      </c>
-      <c r="AA37" s="19">
+        <v>4.5412888806734246</v>
+      </c>
+      <c r="AF37" s="2">
         <f t="shared" si="7"/>
-        <v>0.42403707270153634</v>
-      </c>
-      <c r="AB37" s="19">
+        <v>1.0173788421215519</v>
+      </c>
+      <c r="AG37" s="6">
         <f t="shared" si="8"/>
-        <v>0.32050019789924106</v>
-      </c>
-      <c r="AC37" s="19">
-        <f t="shared" si="9"/>
-        <v>0.74453727060077735</v>
-      </c>
-      <c r="AD37">
-        <f t="shared" si="10"/>
-        <v>4.6202112231590071</v>
-      </c>
-      <c r="AE37">
-        <f t="shared" si="11"/>
-        <v>4.5412888806734246</v>
-      </c>
-      <c r="AF37">
-        <f t="shared" si="12"/>
-        <v>1.0173788421215519</v>
-      </c>
-      <c r="AG37">
-        <f t="shared" si="13"/>
         <v>44.506433965052402</v>
       </c>
       <c r="AK37">
@@ -2982,54 +3223,54 @@
       <c r="T38" t="s">
         <v>68</v>
       </c>
-      <c r="U38" s="24">
+      <c r="U38" s="36">
         <v>50</v>
       </c>
-      <c r="V38" s="24">
+      <c r="V38" s="32">
         <v>66</v>
       </c>
-      <c r="W38" s="24">
-        <f t="shared" ref="W38" si="22">U38/$W$7</f>
+      <c r="W38" s="36">
+        <f>U38/$W$3</f>
         <v>344737.9543387685</v>
       </c>
-      <c r="X38" s="24">
-        <f t="shared" ref="X38" si="23">V38/$W$7</f>
+      <c r="X38" s="32">
+        <f>V38/$W$3</f>
         <v>455054.09972717444</v>
       </c>
-      <c r="Y38" s="22">
+      <c r="Y38" s="37">
+        <f t="shared" si="0"/>
+        <v>23.029119382806488</v>
+      </c>
+      <c r="Z38" s="40">
+        <f t="shared" si="1"/>
+        <v>19.027522851769792</v>
+      </c>
+      <c r="AA38" s="38">
+        <f t="shared" si="2"/>
+        <v>0.49561938814315853</v>
+      </c>
+      <c r="AB38" s="41">
+        <f t="shared" si="3"/>
+        <v>0.43038757702453012</v>
+      </c>
+      <c r="AC38" s="42">
+        <f t="shared" si="4"/>
+        <v>0.92600696516768866</v>
+      </c>
+      <c r="AD38" s="39">
         <f t="shared" si="5"/>
-        <v>23.029119382806488</v>
-      </c>
-      <c r="Z38" s="22">
+        <v>6.3117639660642144</v>
+      </c>
+      <c r="AE38" s="3">
         <f t="shared" si="6"/>
-        <v>19.027522851769792</v>
-      </c>
-      <c r="AA38" s="19">
+        <v>8.1892094569520779</v>
+      </c>
+      <c r="AF38" s="2">
         <f t="shared" si="7"/>
-        <v>0.49561938814315853</v>
-      </c>
-      <c r="AB38" s="19">
+        <v>0.77074154706178133</v>
+      </c>
+      <c r="AG38" s="6">
         <f t="shared" si="8"/>
-        <v>0.43038757702453012</v>
-      </c>
-      <c r="AC38" s="19">
-        <f t="shared" si="9"/>
-        <v>0.92600696516768866</v>
-      </c>
-      <c r="AD38">
-        <f t="shared" si="10"/>
-        <v>6.3117639660642144</v>
-      </c>
-      <c r="AE38">
-        <f t="shared" si="11"/>
-        <v>8.1892094569520779</v>
-      </c>
-      <c r="AF38">
-        <f t="shared" si="12"/>
-        <v>0.77074154706178133</v>
-      </c>
-      <c r="AG38">
-        <f t="shared" si="13"/>
         <v>52.377065352719974</v>
       </c>
     </row>
@@ -3070,61 +3311,61 @@
     </row>
     <row r="40" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C40" s="1"/>
-      <c r="T40" s="28" t="s">
+      <c r="T40" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="U40" s="29">
+      <c r="U40" s="28">
         <v>50</v>
       </c>
-      <c r="V40" s="30">
+      <c r="V40" s="29">
         <v>66</v>
       </c>
-      <c r="W40" s="30">
-        <f t="shared" ref="W40" si="24">U40/$W$7</f>
+      <c r="W40" s="65">
+        <f>U40/$W$3</f>
         <v>344737.9543387685</v>
       </c>
-      <c r="X40" s="30">
-        <f t="shared" ref="X40" si="25">V40/$W$7</f>
+      <c r="X40" s="65">
+        <f>V40/$W$3</f>
         <v>455054.09972717444</v>
       </c>
-      <c r="Y40" s="31">
+      <c r="Y40" s="30">
         <f>SQRT((2*W40)/(kl_annulus*density_IPA))</f>
         <v>24.57618055235416</v>
       </c>
-      <c r="Z40" s="31">
+      <c r="Z40" s="30">
         <f>SQRT((2*X40)/(kl_pintle*density_LOX))</f>
         <v>17.810424718337124</v>
       </c>
-      <c r="AA40" s="32">
+      <c r="AA40" s="31">
         <f>Y40*Density_h20*Annulus_area</f>
         <v>0.52891434386967728</v>
       </c>
-      <c r="AB40" s="32">
+      <c r="AB40" s="31">
         <f>Z40*Density_h20*Pintle_Area</f>
         <v>0.40285777607619272</v>
       </c>
-      <c r="AC40" s="32">
+      <c r="AC40" s="31">
         <f>AB40+AA40</f>
         <v>0.93177211994586995</v>
       </c>
-      <c r="AD40" s="28">
-        <f>(blockage_factor*AA40)*Y40</f>
-        <v>7.1882780096541321</v>
-      </c>
-      <c r="AE40" s="28">
-        <f>AB40*Z40</f>
-        <v>7.1750680930017454</v>
-      </c>
-      <c r="AF40" s="28">
+      <c r="AD40" s="66">
+        <f>density_IPA*gap*orifice*Y40^2</f>
+        <v>0.56335919461680906</v>
+      </c>
+      <c r="AE40" s="66">
+        <f>(AB40*Z40)/12</f>
+        <v>0.59792234108347875</v>
+      </c>
+      <c r="AF40" s="31">
         <f>AD40/AE40</f>
-        <v>1.0018410858937035</v>
-      </c>
-      <c r="AG40" s="28">
+        <v>0.9421945893440965</v>
+      </c>
+      <c r="AG40" s="31">
         <f>ATAN(AE40/AD40)*180/PI()</f>
-        <v>44.947305296892942</v>
-      </c>
-      <c r="AH40" s="24"/>
-      <c r="AI40" s="24"/>
+        <v>46.704787275487071</v>
+      </c>
+      <c r="AH40" s="23"/>
+      <c r="AI40" s="23"/>
       <c r="AK40">
         <f>density_IPA*Y40^2*annulus_area2</f>
         <v>0.56335919461680906</v>
@@ -3613,10 +3854,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="AD27:AF27"/>
     <mergeCell ref="E11:R11"/>
     <mergeCell ref="U9:V9"/>
+    <mergeCell ref="W1:AG1"/>
+    <mergeCell ref="W4:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>